<commit_message>
actualizar el cálculo de las cutoffs
</commit_message>
<xml_diff>
--- a/Contribuciones de bandas espectrales.xlsx
+++ b/Contribuciones de bandas espectrales.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="189">
   <si>
     <t xml:space="preserve">codigo</t>
   </si>
@@ -38,6 +38,15 @@
   </si>
   <si>
     <t xml:space="preserve">HF dividido LF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VLF_cutoff</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LF_cutoff</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HF_cutoff</t>
   </si>
   <si>
     <t xml:space="preserve">r0_promedio</t>
@@ -679,13 +688,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F181"/>
+  <dimension ref="A1:I181"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I158" activeCellId="0" sqref="I158"/>
+      <selection pane="topLeft" activeCell="K4" activeCellId="0" sqref="K4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.84"/>
@@ -710,10 +719,19 @@
       <c r="F1" s="0" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>0</v>
@@ -730,10 +748,19 @@
       <c r="F2" s="1" t="n">
         <v>0.24324542</v>
       </c>
+      <c r="G2" s="1" t="n">
+        <v>0.023224777</v>
+      </c>
+      <c r="H2" s="1" t="n">
+        <v>0.068860191</v>
+      </c>
+      <c r="I2" s="1" t="n">
+        <v>0.17198958</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>0.083</v>
@@ -750,10 +777,19 @@
       <c r="F3" s="1" t="n">
         <v>2.2958383</v>
       </c>
+      <c r="G3" s="1" t="n">
+        <v>0.047372932</v>
+      </c>
+      <c r="H3" s="1" t="n">
+        <v>0.12389438</v>
+      </c>
+      <c r="I3" s="1" t="n">
+        <v>1.0523419</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>0.083</v>
@@ -770,10 +806,19 @@
       <c r="F4" s="1" t="n">
         <v>8.458829</v>
       </c>
+      <c r="G4" s="1" t="n">
+        <v>0.13124116</v>
+      </c>
+      <c r="H4" s="1" t="n">
+        <v>0.15993311</v>
+      </c>
+      <c r="I4" s="1" t="n">
+        <v>1.3435386</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>0.083</v>
@@ -790,10 +835,19 @@
       <c r="F5" s="1" t="n">
         <v>3.5681762</v>
       </c>
+      <c r="G5" s="1" t="n">
+        <v>0.075225631</v>
+      </c>
+      <c r="H5" s="1" t="n">
+        <v>0.13714293</v>
+      </c>
+      <c r="I5" s="1" t="n">
+        <v>1.3107968</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>0.083</v>
@@ -810,10 +864,19 @@
       <c r="F6" s="1" t="n">
         <v>0.35959897</v>
       </c>
+      <c r="G6" s="1" t="n">
+        <v>0.053716222</v>
+      </c>
+      <c r="H6" s="1" t="n">
+        <v>0.14015245</v>
+      </c>
+      <c r="I6" s="1" t="n">
+        <v>0.41015082</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>0.083</v>
@@ -830,10 +893,19 @@
       <c r="F7" s="1" t="n">
         <v>8.0689164</v>
       </c>
+      <c r="G7" s="1" t="n">
+        <v>0.081526817</v>
+      </c>
+      <c r="H7" s="1" t="n">
+        <v>0.13317946</v>
+      </c>
+      <c r="I7" s="1" t="n">
+        <v>2.2036629</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>0.083</v>
@@ -850,10 +922,19 @@
       <c r="F8" s="1" t="n">
         <v>2.5666204</v>
       </c>
+      <c r="G8" s="1" t="n">
+        <v>0.11523166</v>
+      </c>
+      <c r="H8" s="1" t="n">
+        <v>0.20007121</v>
+      </c>
+      <c r="I8" s="1" t="n">
+        <v>1.4159419</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>0.083</v>
@@ -870,10 +951,19 @@
       <c r="F9" s="1" t="n">
         <v>0.97099366</v>
       </c>
+      <c r="G9" s="1" t="n">
+        <v>0.045345312</v>
+      </c>
+      <c r="H9" s="1" t="n">
+        <v>0.12881026</v>
+      </c>
+      <c r="I9" s="1" t="n">
+        <v>0.6053063</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>0.083</v>
@@ -890,10 +980,19 @@
       <c r="F10" s="1" t="n">
         <v>0.52215464</v>
       </c>
+      <c r="G10" s="1" t="n">
+        <v>0.052394242</v>
+      </c>
+      <c r="H10" s="1" t="n">
+        <v>0.15050846</v>
+      </c>
+      <c r="I10" s="1" t="n">
+        <v>0.59555365</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>0.17</v>
@@ -910,10 +1009,19 @@
       <c r="F11" s="1" t="n">
         <v>0.56394305</v>
       </c>
+      <c r="G11" s="1" t="n">
+        <v>0.039680186</v>
+      </c>
+      <c r="H11" s="1" t="n">
+        <v>0.14468417</v>
+      </c>
+      <c r="I11" s="1" t="n">
+        <v>0.65254666</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>0.17</v>
@@ -930,10 +1038,19 @@
       <c r="F12" s="1" t="n">
         <v>0.7048226</v>
       </c>
+      <c r="G12" s="1" t="n">
+        <v>0.040802728</v>
+      </c>
+      <c r="H12" s="1" t="n">
+        <v>0.12500351</v>
+      </c>
+      <c r="I12" s="1" t="n">
+        <v>0.62147219</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>0.17</v>
@@ -950,10 +1067,19 @@
       <c r="F13" s="1" t="n">
         <v>2.414968</v>
       </c>
+      <c r="G13" s="1" t="n">
+        <v>0.056694177</v>
+      </c>
+      <c r="H13" s="1" t="n">
+        <v>0.1329549</v>
+      </c>
+      <c r="I13" s="1" t="n">
+        <v>1.1500437</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>0.17</v>
@@ -970,10 +1096,19 @@
       <c r="F14" s="1" t="n">
         <v>0.74468976</v>
       </c>
+      <c r="G14" s="1" t="n">
+        <v>0.041439276</v>
+      </c>
+      <c r="H14" s="1" t="n">
+        <v>0.14466245</v>
+      </c>
+      <c r="I14" s="1" t="n">
+        <v>0.87556355</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>0.17</v>
@@ -990,10 +1125,19 @@
       <c r="F15" s="1" t="n">
         <v>0.33620442</v>
       </c>
+      <c r="G15" s="1" t="n">
+        <v>0.028052226</v>
+      </c>
+      <c r="H15" s="1" t="n">
+        <v>0.15010037</v>
+      </c>
+      <c r="I15" s="1" t="n">
+        <v>0.98256803</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>0.17</v>
@@ -1010,10 +1154,19 @@
       <c r="F16" s="1" t="n">
         <v>2.0391105</v>
       </c>
+      <c r="G16" s="1" t="n">
+        <v>0.070171417</v>
+      </c>
+      <c r="H16" s="1" t="n">
+        <v>0.16856133</v>
+      </c>
+      <c r="I16" s="1" t="n">
+        <v>1.8353681</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>0.17</v>
@@ -1030,10 +1183,19 @@
       <c r="F17" s="1" t="n">
         <v>0.71566067</v>
       </c>
+      <c r="G17" s="1" t="n">
+        <v>0.039968405</v>
+      </c>
+      <c r="H17" s="1" t="n">
+        <v>0.17517406</v>
+      </c>
+      <c r="I17" s="1" t="n">
+        <v>1.9742684</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>0.25</v>
@@ -1050,10 +1212,19 @@
       <c r="F18" s="1" t="n">
         <v>0.48690541</v>
       </c>
+      <c r="G18" s="1" t="n">
+        <v>0.066387893</v>
+      </c>
+      <c r="H18" s="1" t="n">
+        <v>0.14028316</v>
+      </c>
+      <c r="I18" s="1" t="n">
+        <v>0.41093541</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>0.25</v>
@@ -1070,10 +1241,19 @@
       <c r="F19" s="1" t="n">
         <v>1.3145363</v>
       </c>
+      <c r="G19" s="1" t="n">
+        <v>0.053605195</v>
+      </c>
+      <c r="H19" s="1" t="n">
+        <v>0.10365443</v>
+      </c>
+      <c r="I19" s="1" t="n">
+        <v>0.4715299</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>0.25</v>
@@ -1090,10 +1270,19 @@
       <c r="F20" s="1" t="n">
         <v>2.9301231</v>
       </c>
+      <c r="G20" s="1" t="n">
+        <v>0.077158722</v>
+      </c>
+      <c r="H20" s="1" t="n">
+        <v>0.13257157</v>
+      </c>
+      <c r="I20" s="1" t="n">
+        <v>0.82585785</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>0.25</v>
@@ -1110,10 +1299,19 @@
       <c r="F21" s="1" t="n">
         <v>3.0862586</v>
       </c>
+      <c r="G21" s="1" t="n">
+        <v>0.080977889</v>
+      </c>
+      <c r="H21" s="1" t="n">
+        <v>0.1617675</v>
+      </c>
+      <c r="I21" s="1" t="n">
+        <v>1.0928874</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>0.25</v>
@@ -1130,10 +1328,19 @@
       <c r="F22" s="1" t="n">
         <v>0.43931725</v>
       </c>
+      <c r="G22" s="1" t="n">
+        <v>0.032166958</v>
+      </c>
+      <c r="H22" s="1" t="n">
+        <v>0.17101497</v>
+      </c>
+      <c r="I22" s="1" t="n">
+        <v>1.0698601</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>0.33</v>
@@ -1150,10 +1357,19 @@
       <c r="F23" s="1" t="n">
         <v>0.65386445</v>
       </c>
+      <c r="G23" s="1" t="n">
+        <v>0.043290176</v>
+      </c>
+      <c r="H23" s="1" t="n">
+        <v>0.17065609</v>
+      </c>
+      <c r="I23" s="1" t="n">
+        <v>1.1336096</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B24" s="0" t="n">
         <v>0.33</v>
@@ -1170,10 +1386,19 @@
       <c r="F24" s="1" t="n">
         <v>1.6149609</v>
       </c>
+      <c r="G24" s="1" t="n">
+        <v>0.072309535</v>
+      </c>
+      <c r="H24" s="1" t="n">
+        <v>0.15036474</v>
+      </c>
+      <c r="I24" s="1" t="n">
+        <v>1.0475668</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B25" s="0" t="n">
         <v>0.33</v>
@@ -1190,10 +1415,19 @@
       <c r="F25" s="1" t="n">
         <v>2.3642278</v>
       </c>
+      <c r="G25" s="1" t="n">
+        <v>0.061911726</v>
+      </c>
+      <c r="H25" s="1" t="n">
+        <v>0.18114189</v>
+      </c>
+      <c r="I25" s="1" t="n">
+        <v>0.95426184</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B26" s="0" t="n">
         <v>0.33</v>
@@ -1210,10 +1444,19 @@
       <c r="F26" s="1" t="n">
         <v>1.2854332</v>
       </c>
+      <c r="G26" s="1" t="n">
+        <v>0.030774735</v>
+      </c>
+      <c r="H26" s="1" t="n">
+        <v>0.13076477</v>
+      </c>
+      <c r="I26" s="1" t="n">
+        <v>0.99617222</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B27" s="0" t="n">
         <v>0.33</v>
@@ -1230,10 +1473,19 @@
       <c r="F27" s="1" t="n">
         <v>0.34621818</v>
       </c>
+      <c r="G27" s="1" t="n">
+        <v>0.027874514</v>
+      </c>
+      <c r="H27" s="1" t="n">
+        <v>0.16036118</v>
+      </c>
+      <c r="I27" s="1" t="n">
+        <v>1.0883217</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B28" s="0" t="n">
         <v>0.33</v>
@@ -1250,10 +1502,19 @@
       <c r="F28" s="1" t="n">
         <v>4.2268497</v>
       </c>
+      <c r="G28" s="1" t="n">
+        <v>0.066333397</v>
+      </c>
+      <c r="H28" s="1" t="n">
+        <v>0.12206326</v>
+      </c>
+      <c r="I28" s="1" t="n">
+        <v>1.1307829</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B29" s="0" t="n">
         <v>0.33</v>
@@ -1270,10 +1531,19 @@
       <c r="F29" s="1" t="n">
         <v>0.3936343</v>
       </c>
+      <c r="G29" s="1" t="n">
+        <v>0.025523959</v>
+      </c>
+      <c r="H29" s="1" t="n">
+        <v>0.1580567</v>
+      </c>
+      <c r="I29" s="1" t="n">
+        <v>0.90083063</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B30" s="0" t="n">
         <v>0.33</v>
@@ -1290,10 +1560,19 @@
       <c r="F30" s="1" t="n">
         <v>2.3011211</v>
       </c>
+      <c r="G30" s="1" t="n">
+        <v>0.10633228</v>
+      </c>
+      <c r="H30" s="1" t="n">
+        <v>0.22599034</v>
+      </c>
+      <c r="I30" s="1" t="n">
+        <v>1.0878218</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B31" s="0" t="n">
         <v>0.42</v>
@@ -1310,10 +1589,19 @@
       <c r="F31" s="1" t="n">
         <v>0.36032317</v>
       </c>
+      <c r="G31" s="1" t="n">
+        <v>0.046571985</v>
+      </c>
+      <c r="H31" s="1" t="n">
+        <v>0.20890561</v>
+      </c>
+      <c r="I31" s="1" t="n">
+        <v>0.67006565</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B32" s="0" t="n">
         <v>0.42</v>
@@ -1330,10 +1618,19 @@
       <c r="F32" s="1" t="n">
         <v>0.85602881</v>
       </c>
+      <c r="G32" s="1" t="n">
+        <v>0.063561432</v>
+      </c>
+      <c r="H32" s="1" t="n">
+        <v>0.17407943</v>
+      </c>
+      <c r="I32" s="1" t="n">
+        <v>1.0349614</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B33" s="0" t="n">
         <v>0.42</v>
@@ -1350,10 +1647,19 @@
       <c r="F33" s="1" t="n">
         <v>2.0809745</v>
       </c>
+      <c r="G33" s="1" t="n">
+        <v>0.096787967</v>
+      </c>
+      <c r="H33" s="1" t="n">
+        <v>0.2426782</v>
+      </c>
+      <c r="I33" s="1" t="n">
+        <v>1.0606644</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B34" s="0" t="n">
         <v>0.42</v>
@@ -1370,10 +1676,19 @@
       <c r="F34" s="1" t="n">
         <v>0.90306887</v>
       </c>
+      <c r="G34" s="1" t="n">
+        <v>0.03611071</v>
+      </c>
+      <c r="H34" s="1" t="n">
+        <v>0.16079471</v>
+      </c>
+      <c r="I34" s="1" t="n">
+        <v>1.0523343</v>
+      </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B35" s="0" t="n">
         <v>0.42</v>
@@ -1390,10 +1705,19 @@
       <c r="F35" s="1" t="n">
         <v>1.4315584</v>
       </c>
+      <c r="G35" s="1" t="n">
+        <v>0.064546192</v>
+      </c>
+      <c r="H35" s="1" t="n">
+        <v>0.13702414</v>
+      </c>
+      <c r="I35" s="1" t="n">
+        <v>0.86640184</v>
+      </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B36" s="0" t="n">
         <v>0.42</v>
@@ -1410,10 +1734,19 @@
       <c r="F36" s="1" t="n">
         <v>3.1114739</v>
       </c>
+      <c r="G36" s="1" t="n">
+        <v>0.061991479</v>
+      </c>
+      <c r="H36" s="1" t="n">
+        <v>0.14067286</v>
+      </c>
+      <c r="I36" s="1" t="n">
+        <v>1.182581</v>
+      </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B37" s="0" t="n">
         <v>0.42</v>
@@ -1430,10 +1763,19 @@
       <c r="F37" s="1" t="n">
         <v>1.1091283</v>
       </c>
+      <c r="G37" s="1" t="n">
+        <v>0.12395172</v>
+      </c>
+      <c r="H37" s="1" t="n">
+        <v>0.28359108</v>
+      </c>
+      <c r="I37" s="1" t="n">
+        <v>0.93010221</v>
+      </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B38" s="0" t="n">
         <v>0.42</v>
@@ -1450,10 +1792,19 @@
       <c r="F38" s="1" t="n">
         <v>1.9876913</v>
       </c>
+      <c r="G38" s="1" t="n">
+        <v>0.10339349</v>
+      </c>
+      <c r="H38" s="1" t="n">
+        <v>0.18750579</v>
+      </c>
+      <c r="I38" s="1" t="n">
+        <v>1.3460445</v>
+      </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B39" s="0" t="n">
         <v>0.42</v>
@@ -1470,10 +1821,19 @@
       <c r="F39" s="1" t="n">
         <v>0.51986426</v>
       </c>
+      <c r="G39" s="1" t="n">
+        <v>0.037715208</v>
+      </c>
+      <c r="H39" s="1" t="n">
+        <v>0.23393069</v>
+      </c>
+      <c r="I39" s="1" t="n">
+        <v>0.65475097</v>
+      </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B40" s="0" t="n">
         <v>0.42</v>
@@ -1490,10 +1850,19 @@
       <c r="F40" s="1" t="n">
         <v>0.4162399</v>
       </c>
+      <c r="G40" s="1" t="n">
+        <v>0.030998249</v>
+      </c>
+      <c r="H40" s="1" t="n">
+        <v>0.17567657</v>
+      </c>
+      <c r="I40" s="1" t="n">
+        <v>0.66505787</v>
+      </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B41" s="0" t="n">
         <v>0.42</v>
@@ -1510,10 +1879,19 @@
       <c r="F41" s="1" t="n">
         <v>0.45316464</v>
       </c>
+      <c r="G41" s="1" t="n">
+        <v>0.064127804</v>
+      </c>
+      <c r="H41" s="1" t="n">
+        <v>0.14297573</v>
+      </c>
+      <c r="I41" s="1" t="n">
+        <v>0.37740608</v>
+      </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B42" s="0" t="n">
         <v>0.42</v>
@@ -1530,10 +1908,19 @@
       <c r="F42" s="1" t="n">
         <v>0.73514899</v>
       </c>
+      <c r="G42" s="1" t="n">
+        <v>0.070598025</v>
+      </c>
+      <c r="H42" s="1" t="n">
+        <v>0.29462559</v>
+      </c>
+      <c r="I42" s="1" t="n">
+        <v>0.6750946</v>
+      </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B43" s="0" t="n">
         <v>0.42</v>
@@ -1550,10 +1937,19 @@
       <c r="F43" s="1" t="n">
         <v>0.68890836</v>
       </c>
+      <c r="G43" s="1" t="n">
+        <v>0.042599672</v>
+      </c>
+      <c r="H43" s="1" t="n">
+        <v>0.17354976</v>
+      </c>
+      <c r="I43" s="1" t="n">
+        <v>1.4497127</v>
+      </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B44" s="0" t="n">
         <v>0.5</v>
@@ -1570,10 +1966,19 @@
       <c r="F44" s="1" t="n">
         <v>1.4329746</v>
       </c>
+      <c r="G44" s="1" t="n">
+        <v>0.031797096</v>
+      </c>
+      <c r="H44" s="1" t="n">
+        <v>0.12485237</v>
+      </c>
+      <c r="I44" s="1" t="n">
+        <v>1.062965</v>
+      </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B45" s="0" t="n">
         <v>0.5</v>
@@ -1590,10 +1995,19 @@
       <c r="F45" s="1" t="n">
         <v>1.1504785</v>
       </c>
+      <c r="G45" s="1" t="n">
+        <v>0.073457975</v>
+      </c>
+      <c r="H45" s="1" t="n">
+        <v>0.33245964</v>
+      </c>
+      <c r="I45" s="1" t="n">
+        <v>0.51742047</v>
+      </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B46" s="0" t="n">
         <v>0.5</v>
@@ -1610,10 +2024,19 @@
       <c r="F46" s="1" t="n">
         <v>5.4632933</v>
       </c>
+      <c r="G46" s="1" t="n">
+        <v>0.067563458</v>
+      </c>
+      <c r="H46" s="1" t="n">
+        <v>0.10882361</v>
+      </c>
+      <c r="I46" s="1" t="n">
+        <v>0.92372342</v>
+      </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B47" s="0" t="n">
         <v>0.5</v>
@@ -1630,10 +2053,19 @@
       <c r="F47" s="1" t="n">
         <v>3.5122938</v>
       </c>
+      <c r="G47" s="1" t="n">
+        <v>0.067616511</v>
+      </c>
+      <c r="H47" s="1" t="n">
+        <v>0.1291035</v>
+      </c>
+      <c r="I47" s="1" t="n">
+        <v>1.0250434</v>
+      </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B48" s="0" t="n">
         <v>0.5</v>
@@ -1650,10 +2082,19 @@
       <c r="F48" s="1" t="n">
         <v>0.99924456</v>
       </c>
+      <c r="G48" s="1" t="n">
+        <v>0.04886976</v>
+      </c>
+      <c r="H48" s="1" t="n">
+        <v>0.22055718</v>
+      </c>
+      <c r="I48" s="1" t="n">
+        <v>0.79425865</v>
+      </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="B49" s="0" t="n">
         <v>0.5</v>
@@ -1670,10 +2111,19 @@
       <c r="F49" s="1" t="n">
         <v>0.96981058</v>
       </c>
+      <c r="G49" s="1" t="n">
+        <v>0.070888626</v>
+      </c>
+      <c r="H49" s="1" t="n">
+        <v>0.20980863</v>
+      </c>
+      <c r="I49" s="1" t="n">
+        <v>0.85310439</v>
+      </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B50" s="0" t="n">
         <v>0.58</v>
@@ -1690,10 +2140,19 @@
       <c r="F50" s="1" t="n">
         <v>2.8771151</v>
       </c>
+      <c r="G50" s="1" t="n">
+        <v>0.0323154</v>
+      </c>
+      <c r="H50" s="1" t="n">
+        <v>0.096148871</v>
+      </c>
+      <c r="I50" s="1" t="n">
+        <v>0.80254955</v>
+      </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B51" s="0" t="n">
         <v>0.58</v>
@@ -1710,10 +2169,19 @@
       <c r="F51" s="1" t="n">
         <v>1.9483088</v>
       </c>
+      <c r="G51" s="1" t="n">
+        <v>0.054474563</v>
+      </c>
+      <c r="H51" s="1" t="n">
+        <v>0.18158952</v>
+      </c>
+      <c r="I51" s="1" t="n">
+        <v>1.0228237</v>
+      </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B52" s="0" t="n">
         <v>0.58</v>
@@ -1730,10 +2198,19 @@
       <c r="F52" s="1" t="n">
         <v>0.48383985</v>
       </c>
+      <c r="G52" s="1" t="n">
+        <v>0.075264984</v>
+      </c>
+      <c r="H52" s="1" t="n">
+        <v>0.35291028</v>
+      </c>
+      <c r="I52" s="1" t="n">
+        <v>0.48089735</v>
+      </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B53" s="0" t="n">
         <v>0.58</v>
@@ -1750,10 +2227,19 @@
       <c r="F53" s="1" t="n">
         <v>0.69500508</v>
       </c>
+      <c r="G53" s="1" t="n">
+        <v>0.074418593</v>
+      </c>
+      <c r="H53" s="1" t="n">
+        <v>0.32432674</v>
+      </c>
+      <c r="I53" s="1" t="n">
+        <v>0.7092341</v>
+      </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B54" s="0" t="n">
         <v>0.58</v>
@@ -1770,10 +2256,19 @@
       <c r="F54" s="1" t="n">
         <v>0.68207204</v>
       </c>
+      <c r="G54" s="1" t="n">
+        <v>0.027503831</v>
+      </c>
+      <c r="H54" s="1" t="n">
+        <v>0.15769271</v>
+      </c>
+      <c r="I54" s="1" t="n">
+        <v>0.84928832</v>
+      </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B55" s="0" t="n">
         <v>0.58</v>
@@ -1790,10 +2285,19 @@
       <c r="F55" s="1" t="n">
         <v>1.4651016</v>
       </c>
+      <c r="G55" s="1" t="n">
+        <v>0.083604914</v>
+      </c>
+      <c r="H55" s="1" t="n">
+        <v>0.22854655</v>
+      </c>
+      <c r="I55" s="1" t="n">
+        <v>0.5571123</v>
+      </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B56" s="0" t="n">
         <v>0.67</v>
@@ -1810,10 +2314,19 @@
       <c r="F56" s="1" t="n">
         <v>1.7934416</v>
       </c>
+      <c r="G56" s="1" t="n">
+        <v>0.066540749</v>
+      </c>
+      <c r="H56" s="1" t="n">
+        <v>0.19514629</v>
+      </c>
+      <c r="I56" s="1" t="n">
+        <v>0.98491585</v>
+      </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B57" s="0" t="n">
         <v>0.67</v>
@@ -1830,10 +2343,19 @@
       <c r="F57" s="1" t="n">
         <v>2.8555367</v>
       </c>
+      <c r="G57" s="1" t="n">
+        <v>0.064834754</v>
+      </c>
+      <c r="H57" s="1" t="n">
+        <v>0.13234909</v>
+      </c>
+      <c r="I57" s="1" t="n">
+        <v>1.1832742</v>
+      </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B58" s="0" t="n">
         <v>0.67</v>
@@ -1850,10 +2372,19 @@
       <c r="F58" s="1" t="n">
         <v>0.90631025</v>
       </c>
+      <c r="G58" s="1" t="n">
+        <v>0.054661637</v>
+      </c>
+      <c r="H58" s="1" t="n">
+        <v>0.25127045</v>
+      </c>
+      <c r="I58" s="1" t="n">
+        <v>0.8780392</v>
+      </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B59" s="0" t="n">
         <v>0.67</v>
@@ -1870,10 +2401,19 @@
       <c r="F59" s="1" t="n">
         <v>1.2934526</v>
       </c>
+      <c r="G59" s="1" t="n">
+        <v>0.064127667</v>
+      </c>
+      <c r="H59" s="1" t="n">
+        <v>0.27284205</v>
+      </c>
+      <c r="I59" s="1" t="n">
+        <v>0.7577746</v>
+      </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="B60" s="0" t="n">
         <v>0.67</v>
@@ -1890,10 +2430,19 @@
       <c r="F60" s="1" t="n">
         <v>1.4398214</v>
       </c>
+      <c r="G60" s="1" t="n">
+        <v>0.12128661</v>
+      </c>
+      <c r="H60" s="1" t="n">
+        <v>0.24069875</v>
+      </c>
+      <c r="I60" s="1" t="n">
+        <v>1.0986774</v>
+      </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="B61" s="0" t="n">
         <v>0.75</v>
@@ -1910,10 +2459,19 @@
       <c r="F61" s="1" t="n">
         <v>2.1560719</v>
       </c>
+      <c r="G61" s="1" t="n">
+        <v>0.072014243</v>
+      </c>
+      <c r="H61" s="1" t="n">
+        <v>0.13805497</v>
+      </c>
+      <c r="I61" s="1" t="n">
+        <v>1.0356803</v>
+      </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B62" s="0" t="n">
         <v>0.75</v>
@@ -1930,10 +2488,19 @@
       <c r="F62" s="1" t="n">
         <v>3.5861811</v>
       </c>
+      <c r="G62" s="1" t="n">
+        <v>0.11527401</v>
+      </c>
+      <c r="H62" s="1" t="n">
+        <v>0.20495952</v>
+      </c>
+      <c r="I62" s="1" t="n">
+        <v>1.1458602</v>
+      </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B63" s="0" t="n">
         <v>0.75</v>
@@ -1950,10 +2517,19 @@
       <c r="F63" s="1" t="n">
         <v>1.1104814</v>
       </c>
+      <c r="G63" s="1" t="n">
+        <v>0.073208543</v>
+      </c>
+      <c r="H63" s="1" t="n">
+        <v>0.31223611</v>
+      </c>
+      <c r="I63" s="1" t="n">
+        <v>0.5894292</v>
+      </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="B64" s="0" t="n">
         <v>0.75</v>
@@ -1970,10 +2546,19 @@
       <c r="F64" s="1" t="n">
         <v>5.1956612</v>
       </c>
+      <c r="G64" s="1" t="n">
+        <v>0.051715105</v>
+      </c>
+      <c r="H64" s="1" t="n">
+        <v>0.088527048</v>
+      </c>
+      <c r="I64" s="1" t="n">
+        <v>1.0454717</v>
+      </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B65" s="0" t="n">
         <v>0.75</v>
@@ -1990,10 +2575,19 @@
       <c r="F65" s="1" t="n">
         <v>5.6361223</v>
       </c>
+      <c r="G65" s="1" t="n">
+        <v>0.063095307</v>
+      </c>
+      <c r="H65" s="1" t="n">
+        <v>0.10435054</v>
+      </c>
+      <c r="I65" s="1" t="n">
+        <v>0.88789113</v>
+      </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B66" s="0" t="n">
         <v>0.75</v>
@@ -2010,10 +2604,19 @@
       <c r="F66" s="1" t="n">
         <v>0.70296018</v>
       </c>
+      <c r="G66" s="1" t="n">
+        <v>0.054645346</v>
+      </c>
+      <c r="H66" s="1" t="n">
+        <v>0.3219493</v>
+      </c>
+      <c r="I66" s="1" t="n">
+        <v>1.1188114</v>
+      </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="B67" s="0" t="n">
         <v>0.75</v>
@@ -2030,10 +2633,19 @@
       <c r="F67" s="1" t="n">
         <v>0.85534511</v>
       </c>
+      <c r="G67" s="1" t="n">
+        <v>0.083786044</v>
+      </c>
+      <c r="H67" s="1" t="n">
+        <v>0.25780552</v>
+      </c>
+      <c r="I67" s="1" t="n">
+        <v>0.71250707</v>
+      </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="B68" s="0" t="n">
         <v>0.83</v>
@@ -2050,10 +2662,19 @@
       <c r="F68" s="1" t="n">
         <v>1.0740755</v>
       </c>
+      <c r="G68" s="1" t="n">
+        <v>0.09716221</v>
+      </c>
+      <c r="H68" s="1" t="n">
+        <v>0.28681227</v>
+      </c>
+      <c r="I68" s="1" t="n">
+        <v>0.57305558</v>
+      </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B69" s="0" t="n">
         <v>0.83</v>
@@ -2070,10 +2691,19 @@
       <c r="F69" s="1" t="n">
         <v>3.7461523</v>
       </c>
+      <c r="G69" s="1" t="n">
+        <v>0.057971957</v>
+      </c>
+      <c r="H69" s="1" t="n">
+        <v>0.13527199</v>
+      </c>
+      <c r="I69" s="1" t="n">
+        <v>0.92522228</v>
+      </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="B70" s="0" t="n">
         <v>0.83</v>
@@ -2090,10 +2720,19 @@
       <c r="F70" s="1" t="n">
         <v>0.84501395</v>
       </c>
+      <c r="G70" s="1" t="n">
+        <v>0.080542102</v>
+      </c>
+      <c r="H70" s="1" t="n">
+        <v>0.33970768</v>
+      </c>
+      <c r="I70" s="1" t="n">
+        <v>1.006599</v>
+      </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B71" s="0" t="n">
         <v>0.83</v>
@@ -2110,10 +2749,19 @@
       <c r="F71" s="1" t="n">
         <v>3.3678503</v>
       </c>
+      <c r="G71" s="1" t="n">
+        <v>0.031019971</v>
+      </c>
+      <c r="H71" s="1" t="n">
+        <v>0.093722272</v>
+      </c>
+      <c r="I71" s="1" t="n">
+        <v>1.0610425</v>
+      </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="B72" s="0" t="n">
         <v>0.92</v>
@@ -2130,10 +2778,19 @@
       <c r="F72" s="1" t="n">
         <v>1.5434352</v>
       </c>
+      <c r="G72" s="1" t="n">
+        <v>0.050163547</v>
+      </c>
+      <c r="H72" s="1" t="n">
+        <v>0.18153186</v>
+      </c>
+      <c r="I72" s="1" t="n">
+        <v>1.0341202</v>
+      </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B73" s="0" t="n">
         <v>1</v>
@@ -2150,10 +2807,19 @@
       <c r="F73" s="1" t="n">
         <v>0.88640927</v>
       </c>
+      <c r="G73" s="1" t="n">
+        <v>0.088729969</v>
+      </c>
+      <c r="H73" s="1" t="n">
+        <v>0.27687715</v>
+      </c>
+      <c r="I73" s="1" t="n">
+        <v>0.75142428</v>
+      </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="B74" s="0" t="n">
         <v>1</v>
@@ -2170,10 +2836,19 @@
       <c r="F74" s="1" t="n">
         <v>1.3934671</v>
       </c>
+      <c r="G74" s="1" t="n">
+        <v>0.080262952</v>
+      </c>
+      <c r="H74" s="1" t="n">
+        <v>0.21159799</v>
+      </c>
+      <c r="I74" s="1" t="n">
+        <v>0.80224723</v>
+      </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="B75" s="0" t="n">
         <v>1.08</v>
@@ -2190,10 +2865,19 @@
       <c r="F75" s="1" t="n">
         <v>1.6365662</v>
       </c>
+      <c r="G75" s="1" t="n">
+        <v>0.051061719</v>
+      </c>
+      <c r="H75" s="1" t="n">
+        <v>0.16412579</v>
+      </c>
+      <c r="I75" s="1" t="n">
+        <v>0.71561192</v>
+      </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="B76" s="0" t="n">
         <v>1.08</v>
@@ -2210,10 +2894,19 @@
       <c r="F76" s="1" t="n">
         <v>4.4279576</v>
       </c>
+      <c r="G76" s="1" t="n">
+        <v>0.081484137</v>
+      </c>
+      <c r="H76" s="1" t="n">
+        <v>0.14303295</v>
+      </c>
+      <c r="I76" s="1" t="n">
+        <v>0.86046276</v>
+      </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="B77" s="0" t="n">
         <v>1.08</v>
@@ -2230,10 +2923,19 @@
       <c r="F77" s="1" t="n">
         <v>0.69981047</v>
       </c>
+      <c r="G77" s="1" t="n">
+        <v>0.070027685</v>
+      </c>
+      <c r="H77" s="1" t="n">
+        <v>0.34112859</v>
+      </c>
+      <c r="I77" s="1" t="n">
+        <v>1.1627567</v>
+      </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="B78" s="0" t="n">
         <v>1.17</v>
@@ -2250,10 +2952,19 @@
       <c r="F78" s="1" t="n">
         <v>2.8085585</v>
       </c>
+      <c r="G78" s="1" t="n">
+        <v>0.036846376</v>
+      </c>
+      <c r="H78" s="1" t="n">
+        <v>0.13768392</v>
+      </c>
+      <c r="I78" s="1" t="n">
+        <v>1.083858</v>
+      </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B79" s="0" t="n">
         <v>1.17</v>
@@ -2270,10 +2981,19 @@
       <c r="F79" s="1" t="n">
         <v>0.99561919</v>
       </c>
+      <c r="G79" s="1" t="n">
+        <v>0.068697945</v>
+      </c>
+      <c r="H79" s="1" t="n">
+        <v>0.14171077</v>
+      </c>
+      <c r="I79" s="1" t="n">
+        <v>0.50309138</v>
+      </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="B80" s="0" t="n">
         <v>1.5</v>
@@ -2290,10 +3010,19 @@
       <c r="F80" s="1" t="n">
         <v>1.3958598</v>
       </c>
+      <c r="G80" s="1" t="n">
+        <v>0.088045931</v>
+      </c>
+      <c r="H80" s="1" t="n">
+        <v>0.24727046</v>
+      </c>
+      <c r="I80" s="1" t="n">
+        <v>0.47846792</v>
+      </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B81" s="0" t="n">
         <v>1.67</v>
@@ -2310,10 +3039,19 @@
       <c r="F81" s="1" t="n">
         <v>0.24562207</v>
       </c>
+      <c r="G81" s="1" t="n">
+        <v>0.028328409</v>
+      </c>
+      <c r="H81" s="1" t="n">
+        <v>0.35788439</v>
+      </c>
+      <c r="I81" s="1" t="n">
+        <v>0.50238552</v>
+      </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="B82" s="0" t="n">
         <v>1.67</v>
@@ -2330,10 +3068,19 @@
       <c r="F82" s="1" t="n">
         <v>2.7597323</v>
       </c>
+      <c r="G82" s="1" t="n">
+        <v>0.054087417</v>
+      </c>
+      <c r="H82" s="1" t="n">
+        <v>0.13847817</v>
+      </c>
+      <c r="I82" s="1" t="n">
+        <v>1.2022031</v>
+      </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="B83" s="0" t="n">
         <v>1.75</v>
@@ -2350,10 +3097,19 @@
       <c r="F83" s="1" t="n">
         <v>1.1554719</v>
       </c>
+      <c r="G83" s="1" t="n">
+        <v>0.05010786</v>
+      </c>
+      <c r="H83" s="1" t="n">
+        <v>0.20642313</v>
+      </c>
+      <c r="I83" s="1" t="n">
+        <v>0.59256449</v>
+      </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B84" s="0" t="n">
         <v>1.75</v>
@@ -2370,10 +3126,19 @@
       <c r="F84" s="1" t="n">
         <v>1.1852345</v>
       </c>
+      <c r="G84" s="1" t="n">
+        <v>0.05480861</v>
+      </c>
+      <c r="H84" s="1" t="n">
+        <v>0.27812904</v>
+      </c>
+      <c r="I84" s="1" t="n">
+        <v>0.85691273</v>
+      </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="B85" s="0" t="n">
         <v>2.08</v>
@@ -2390,10 +3155,19 @@
       <c r="F85" s="1" t="n">
         <v>0.57265196</v>
       </c>
+      <c r="G85" s="1" t="n">
+        <v>0.043244299</v>
+      </c>
+      <c r="H85" s="1" t="n">
+        <v>0.23873149</v>
+      </c>
+      <c r="I85" s="1" t="n">
+        <v>0.39888685</v>
+      </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="B86" s="0" t="n">
         <v>2.08</v>
@@ -2410,10 +3184,19 @@
       <c r="F86" s="1" t="n">
         <v>2.5676282</v>
       </c>
+      <c r="G86" s="1" t="n">
+        <v>0.041158802</v>
+      </c>
+      <c r="H86" s="1" t="n">
+        <v>0.11867608</v>
+      </c>
+      <c r="I86" s="1" t="n">
+        <v>0.80744145</v>
+      </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="B87" s="0" t="n">
         <v>2.17</v>
@@ -2430,10 +3213,19 @@
       <c r="F87" s="1" t="n">
         <v>1.6865993</v>
       </c>
+      <c r="G87" s="1" t="n">
+        <v>0.045607175</v>
+      </c>
+      <c r="H87" s="1" t="n">
+        <v>0.26017848</v>
+      </c>
+      <c r="I87" s="1" t="n">
+        <v>0.60115549</v>
+      </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="B88" s="0" t="n">
         <v>2.25</v>
@@ -2450,10 +3242,19 @@
       <c r="F88" s="1" t="n">
         <v>3.2274389</v>
       </c>
+      <c r="G88" s="1" t="n">
+        <v>0.046950247</v>
+      </c>
+      <c r="H88" s="1" t="n">
+        <v>0.11937674</v>
+      </c>
+      <c r="I88" s="1" t="n">
+        <v>0.79294587</v>
+      </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B89" s="0" t="n">
         <v>2.5</v>
@@ -2470,10 +3271,19 @@
       <c r="F89" s="1" t="n">
         <v>0.98643898</v>
       </c>
+      <c r="G89" s="1" t="n">
+        <v>0.052455581</v>
+      </c>
+      <c r="H89" s="1" t="n">
+        <v>0.29113755</v>
+      </c>
+      <c r="I89" s="1" t="n">
+        <v>0.49199561</v>
+      </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="B90" s="0" t="n">
         <v>2.58</v>
@@ -2490,10 +3300,19 @@
       <c r="F90" s="1" t="n">
         <v>1.0183608</v>
       </c>
+      <c r="G90" s="1" t="n">
+        <v>0.052838244</v>
+      </c>
+      <c r="H90" s="1" t="n">
+        <v>0.23211549</v>
+      </c>
+      <c r="I90" s="1" t="n">
+        <v>0.48884455</v>
+      </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="B91" s="0" t="n">
         <v>2.67</v>
@@ -2510,10 +3329,19 @@
       <c r="F91" s="1" t="n">
         <v>0.69843628</v>
       </c>
+      <c r="G91" s="1" t="n">
+        <v>0.051988127</v>
+      </c>
+      <c r="H91" s="1" t="n">
+        <v>0.19042404</v>
+      </c>
+      <c r="I91" s="1" t="n">
+        <v>0.47996638</v>
+      </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="B92" s="0" t="n">
         <v>2.75</v>
@@ -2530,10 +3358,19 @@
       <c r="F92" s="1" t="n">
         <v>1.3103889</v>
       </c>
+      <c r="G92" s="1" t="n">
+        <v>0.048287175</v>
+      </c>
+      <c r="H92" s="1" t="n">
+        <v>0.16878899</v>
+      </c>
+      <c r="I92" s="1" t="n">
+        <v>0.34360903</v>
+      </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B93" s="0" t="n">
         <v>2.83</v>
@@ -2550,10 +3387,19 @@
       <c r="F93" s="1" t="n">
         <v>3.3350526</v>
       </c>
+      <c r="G93" s="1" t="n">
+        <v>0.028375551</v>
+      </c>
+      <c r="H93" s="1" t="n">
+        <v>0.084065644</v>
+      </c>
+      <c r="I93" s="1" t="n">
+        <v>0.88674151</v>
+      </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="B94" s="0" t="n">
         <v>2.92</v>
@@ -2570,10 +3416,19 @@
       <c r="F94" s="1" t="n">
         <v>0.69228119</v>
       </c>
+      <c r="G94" s="1" t="n">
+        <v>0.047812023</v>
+      </c>
+      <c r="H94" s="1" t="n">
+        <v>0.22888057</v>
+      </c>
+      <c r="I94" s="1" t="n">
+        <v>0.40167509</v>
+      </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="B95" s="0" t="n">
         <v>3</v>
@@ -2590,10 +3445,19 @@
       <c r="F95" s="1" t="n">
         <v>0.34292837</v>
       </c>
+      <c r="G95" s="1" t="n">
+        <v>0.037611319</v>
+      </c>
+      <c r="H95" s="1" t="n">
+        <v>0.18800906</v>
+      </c>
+      <c r="I95" s="1" t="n">
+        <v>0.65953285</v>
+      </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="B96" s="0" t="n">
         <v>3.42</v>
@@ -2610,10 +3474,19 @@
       <c r="F96" s="1" t="n">
         <v>0.84755473</v>
       </c>
+      <c r="G96" s="1" t="n">
+        <v>0.054589053</v>
+      </c>
+      <c r="H96" s="1" t="n">
+        <v>0.21625033</v>
+      </c>
+      <c r="I96" s="1" t="n">
+        <v>0.34769901</v>
+      </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="B97" s="0" t="n">
         <v>3.42</v>
@@ -2630,10 +3503,19 @@
       <c r="F97" s="1" t="n">
         <v>1.1038948</v>
       </c>
+      <c r="G97" s="1" t="n">
+        <v>0.039664274</v>
+      </c>
+      <c r="H97" s="1" t="n">
+        <v>0.25477005</v>
+      </c>
+      <c r="I97" s="1" t="n">
+        <v>0.4536642</v>
+      </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="B98" s="0" t="n">
         <v>4</v>
@@ -2650,10 +3532,19 @@
       <c r="F98" s="1" t="n">
         <v>1.4773517</v>
       </c>
+      <c r="G98" s="1" t="n">
+        <v>0.05286734</v>
+      </c>
+      <c r="H98" s="1" t="n">
+        <v>0.23425505</v>
+      </c>
+      <c r="I98" s="1" t="n">
+        <v>0.38009152</v>
+      </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="B99" s="0" t="n">
         <v>4.5</v>
@@ -2670,10 +3561,19 @@
       <c r="F99" s="1" t="n">
         <v>0.42473698</v>
       </c>
+      <c r="G99" s="1" t="n">
+        <v>0.043944037</v>
+      </c>
+      <c r="H99" s="1" t="n">
+        <v>0.24586018</v>
+      </c>
+      <c r="I99" s="1" t="n">
+        <v>0.48679074</v>
+      </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="B100" s="0" t="n">
         <v>5</v>
@@ -2690,10 +3590,19 @@
       <c r="F100" s="1" t="n">
         <v>0.67644493</v>
       </c>
+      <c r="G100" s="1" t="n">
+        <v>0.041528326</v>
+      </c>
+      <c r="H100" s="1" t="n">
+        <v>0.20390543</v>
+      </c>
+      <c r="I100" s="1" t="n">
+        <v>0.35583174</v>
+      </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="B101" s="0" t="n">
         <v>5</v>
@@ -2710,10 +3619,19 @@
       <c r="F101" s="1" t="n">
         <v>1.1124172</v>
       </c>
+      <c r="G101" s="1" t="n">
+        <v>0.03999257</v>
+      </c>
+      <c r="H101" s="1" t="n">
+        <v>0.29560683</v>
+      </c>
+      <c r="I101" s="1" t="n">
+        <v>0.45156788</v>
+      </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="B102" s="0" t="n">
         <v>5.17</v>
@@ -2730,10 +3648,19 @@
       <c r="F102" s="1" t="n">
         <v>0.66166001</v>
       </c>
+      <c r="G102" s="1" t="n">
+        <v>0.039345588</v>
+      </c>
+      <c r="H102" s="1" t="n">
+        <v>0.14837016</v>
+      </c>
+      <c r="I102" s="1" t="n">
+        <v>0.70703285</v>
+      </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="B103" s="0" t="n">
         <v>5.42</v>
@@ -2750,10 +3677,19 @@
       <c r="F103" s="1" t="n">
         <v>1.7741407</v>
       </c>
+      <c r="G103" s="1" t="n">
+        <v>0.042224275</v>
+      </c>
+      <c r="H103" s="1" t="n">
+        <v>0.20903527</v>
+      </c>
+      <c r="I103" s="1" t="n">
+        <v>0.3664978</v>
+      </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="B104" s="0" t="n">
         <v>5.83</v>
@@ -2770,10 +3706,19 @@
       <c r="F104" s="1" t="n">
         <v>1.7048217</v>
       </c>
+      <c r="G104" s="1" t="n">
+        <v>0.045572727</v>
+      </c>
+      <c r="H104" s="1" t="n">
+        <v>0.1735203</v>
+      </c>
+      <c r="I104" s="1" t="n">
+        <v>0.32587089</v>
+      </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="B105" s="0" t="n">
         <v>6</v>
@@ -2790,10 +3735,19 @@
       <c r="F105" s="1" t="n">
         <v>1.1072694</v>
       </c>
+      <c r="G105" s="1" t="n">
+        <v>0.039317862</v>
+      </c>
+      <c r="H105" s="1" t="n">
+        <v>0.19256018</v>
+      </c>
+      <c r="I105" s="1" t="n">
+        <v>0.35064907</v>
+      </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="B106" s="0" t="n">
         <v>6</v>
@@ -2810,10 +3764,19 @@
       <c r="F106" s="1" t="n">
         <v>1.2365954</v>
       </c>
+      <c r="G106" s="1" t="n">
+        <v>0.04659632</v>
+      </c>
+      <c r="H106" s="1" t="n">
+        <v>0.17491434</v>
+      </c>
+      <c r="I106" s="1" t="n">
+        <v>0.34097041</v>
+      </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="B107" s="0" t="n">
         <v>7</v>
@@ -2830,10 +3793,19 @@
       <c r="F107" s="1" t="n">
         <v>0.81531027</v>
       </c>
+      <c r="G107" s="1" t="n">
+        <v>0.036760554</v>
+      </c>
+      <c r="H107" s="1" t="n">
+        <v>0.19062991</v>
+      </c>
+      <c r="I107" s="1" t="n">
+        <v>0.45335773</v>
+      </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="B108" s="0" t="n">
         <v>7</v>
@@ -2850,10 +3822,19 @@
       <c r="F108" s="1" t="n">
         <v>1.0228704</v>
       </c>
+      <c r="G108" s="1" t="n">
+        <v>0.037523104</v>
+      </c>
+      <c r="H108" s="1" t="n">
+        <v>0.2209823</v>
+      </c>
+      <c r="I108" s="1" t="n">
+        <v>0.41399832</v>
+      </c>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="B109" s="0" t="n">
         <v>8</v>
@@ -2870,10 +3851,19 @@
       <c r="F109" s="1" t="n">
         <v>0.8009309</v>
       </c>
+      <c r="G109" s="1" t="n">
+        <v>0.048247336</v>
+      </c>
+      <c r="H109" s="1" t="n">
+        <v>0.22976896</v>
+      </c>
+      <c r="I109" s="1" t="n">
+        <v>0.50246033</v>
+      </c>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="B110" s="0" t="n">
         <v>8</v>
@@ -2890,10 +3880,19 @@
       <c r="F110" s="1" t="n">
         <v>0.3358759</v>
       </c>
+      <c r="G110" s="1" t="n">
+        <v>0.042198938</v>
+      </c>
+      <c r="H110" s="1" t="n">
+        <v>0.26615315</v>
+      </c>
+      <c r="I110" s="1" t="n">
+        <v>0.41892454</v>
+      </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="B111" s="0" t="n">
         <v>9</v>
@@ -2910,10 +3909,19 @@
       <c r="F111" s="1" t="n">
         <v>0.59920476</v>
       </c>
+      <c r="G111" s="1" t="n">
+        <v>0.038901254</v>
+      </c>
+      <c r="H111" s="1" t="n">
+        <v>0.18592675</v>
+      </c>
+      <c r="I111" s="1" t="n">
+        <v>0.37498017</v>
+      </c>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="B112" s="0" t="n">
         <v>10</v>
@@ -2930,10 +3938,19 @@
       <c r="F112" s="1" t="n">
         <v>0.29454395</v>
       </c>
+      <c r="G112" s="1" t="n">
+        <v>0.034357412</v>
+      </c>
+      <c r="H112" s="1" t="n">
+        <v>0.2601912</v>
+      </c>
+      <c r="I112" s="1" t="n">
+        <v>0.35459245</v>
+      </c>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="B113" s="0" t="n">
         <v>10</v>
@@ -2950,10 +3967,19 @@
       <c r="F113" s="1" t="n">
         <v>0.86316587</v>
       </c>
+      <c r="G113" s="1" t="n">
+        <v>0.048046757</v>
+      </c>
+      <c r="H113" s="1" t="n">
+        <v>0.16049975</v>
+      </c>
+      <c r="I113" s="1" t="n">
+        <v>0.35585358</v>
+      </c>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="B114" s="0" t="n">
         <v>10</v>
@@ -2970,10 +3996,19 @@
       <c r="F114" s="1" t="n">
         <v>0.89836471</v>
       </c>
+      <c r="G114" s="1" t="n">
+        <v>0.04217051</v>
+      </c>
+      <c r="H114" s="1" t="n">
+        <v>0.18221003</v>
+      </c>
+      <c r="I114" s="1" t="n">
+        <v>0.49345234</v>
+      </c>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="B115" s="0" t="n">
         <v>10</v>
@@ -2990,10 +4025,19 @@
       <c r="F115" s="1" t="n">
         <v>0.50507264</v>
       </c>
+      <c r="G115" s="1" t="n">
+        <v>0.042274148</v>
+      </c>
+      <c r="H115" s="1" t="n">
+        <v>0.22049687</v>
+      </c>
+      <c r="I115" s="1" t="n">
+        <v>0.42574658</v>
+      </c>
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="0" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="B116" s="0" t="n">
         <v>11</v>
@@ -3010,10 +4054,19 @@
       <c r="F116" s="1" t="n">
         <v>0.68400312</v>
       </c>
+      <c r="G116" s="1" t="n">
+        <v>0.051809455</v>
+      </c>
+      <c r="H116" s="1" t="n">
+        <v>0.20339925</v>
+      </c>
+      <c r="I116" s="1" t="n">
+        <v>0.47339337</v>
+      </c>
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="B117" s="0" t="n">
         <v>11</v>
@@ -3030,10 +4083,19 @@
       <c r="F117" s="1" t="n">
         <v>0.38490933</v>
       </c>
+      <c r="G117" s="1" t="n">
+        <v>0.030250249</v>
+      </c>
+      <c r="H117" s="1" t="n">
+        <v>0.1694084</v>
+      </c>
+      <c r="I117" s="1" t="n">
+        <v>0.57213042</v>
+      </c>
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="0" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="B118" s="0" t="n">
         <v>11</v>
@@ -3050,10 +4112,19 @@
       <c r="F118" s="1" t="n">
         <v>0.97690038</v>
       </c>
+      <c r="G118" s="1" t="n">
+        <v>0.049134383</v>
+      </c>
+      <c r="H118" s="1" t="n">
+        <v>0.18737219</v>
+      </c>
+      <c r="I118" s="1" t="n">
+        <v>0.34656235</v>
+      </c>
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="0" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="B119" s="0" t="n">
         <v>11</v>
@@ -3070,10 +4141,19 @@
       <c r="F119" s="1" t="n">
         <v>0.93073863</v>
       </c>
+      <c r="G119" s="1" t="n">
+        <v>0.048575181</v>
+      </c>
+      <c r="H119" s="1" t="n">
+        <v>0.20653842</v>
+      </c>
+      <c r="I119" s="1" t="n">
+        <v>0.38234427</v>
+      </c>
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="0" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="B120" s="0" t="n">
         <v>12</v>
@@ -3090,10 +4170,19 @@
       <c r="F120" s="1" t="n">
         <v>0.56645203</v>
       </c>
+      <c r="G120" s="1" t="n">
+        <v>0.044079659</v>
+      </c>
+      <c r="H120" s="1" t="n">
+        <v>0.23459157</v>
+      </c>
+      <c r="I120" s="1" t="n">
+        <v>0.42089364</v>
+      </c>
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="0" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="B121" s="0" t="n">
         <v>12</v>
@@ -3110,10 +4199,19 @@
       <c r="F121" s="1" t="n">
         <v>1.0123563</v>
       </c>
+      <c r="G121" s="1" t="n">
+        <v>0.044373672</v>
+      </c>
+      <c r="H121" s="1" t="n">
+        <v>0.19293938</v>
+      </c>
+      <c r="I121" s="1" t="n">
+        <v>0.48221979</v>
+      </c>
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="0" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="B122" s="0" t="n">
         <v>12</v>
@@ -3130,10 +4228,19 @@
       <c r="F122" s="1" t="n">
         <v>0.47600861</v>
       </c>
+      <c r="G122" s="1" t="n">
+        <v>0.039285955</v>
+      </c>
+      <c r="H122" s="1" t="n">
+        <v>0.23120735</v>
+      </c>
+      <c r="I122" s="1" t="n">
+        <v>0.4423871</v>
+      </c>
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="0" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="B123" s="0" t="n">
         <v>12</v>
@@ -3150,10 +4257,19 @@
       <c r="F123" s="1" t="n">
         <v>0.98153662</v>
       </c>
+      <c r="G123" s="1" t="n">
+        <v>0.038119793</v>
+      </c>
+      <c r="H123" s="1" t="n">
+        <v>0.20186586</v>
+      </c>
+      <c r="I123" s="1" t="n">
+        <v>0.3561234</v>
+      </c>
     </row>
     <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="0" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="B124" s="0" t="n">
         <v>12</v>
@@ -3170,10 +4286,19 @@
       <c r="F124" s="1" t="n">
         <v>0.8156669</v>
       </c>
+      <c r="G124" s="1" t="n">
+        <v>0.04264023</v>
+      </c>
+      <c r="H124" s="1" t="n">
+        <v>0.19510381</v>
+      </c>
+      <c r="I124" s="1" t="n">
+        <v>0.41189936</v>
+      </c>
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="0" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="B125" s="0" t="n">
         <v>13</v>
@@ -3190,10 +4315,19 @@
       <c r="F125" s="1" t="n">
         <v>0.70859852</v>
       </c>
+      <c r="G125" s="1" t="n">
+        <v>0.044492175</v>
+      </c>
+      <c r="H125" s="1" t="n">
+        <v>0.19261931</v>
+      </c>
+      <c r="I125" s="1" t="n">
+        <v>0.36176202</v>
+      </c>
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="0" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="B126" s="0" t="n">
         <v>13</v>
@@ -3210,10 +4344,19 @@
       <c r="F126" s="1" t="n">
         <v>0.25545537</v>
       </c>
+      <c r="G126" s="1" t="n">
+        <v>0.030883123</v>
+      </c>
+      <c r="H126" s="1" t="n">
+        <v>0.22917828</v>
+      </c>
+      <c r="I126" s="1" t="n">
+        <v>0.3878256</v>
+      </c>
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="0" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="B127" s="0" t="n">
         <v>14</v>
@@ -3230,10 +4373,19 @@
       <c r="F127" s="1" t="n">
         <v>1.0128455</v>
       </c>
+      <c r="G127" s="1" t="n">
+        <v>0.045302747</v>
+      </c>
+      <c r="H127" s="1" t="n">
+        <v>0.1990132</v>
+      </c>
+      <c r="I127" s="1" t="n">
+        <v>0.32133836</v>
+      </c>
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="0" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="B128" s="0" t="n">
         <v>15</v>
@@ -3250,10 +4402,19 @@
       <c r="F128" s="1" t="n">
         <v>0.64653518</v>
       </c>
+      <c r="G128" s="1" t="n">
+        <v>0.053015915</v>
+      </c>
+      <c r="H128" s="1" t="n">
+        <v>0.17936781</v>
+      </c>
+      <c r="I128" s="1" t="n">
+        <v>0.33624612</v>
+      </c>
     </row>
     <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="0" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="B129" s="0" t="n">
         <v>15</v>
@@ -3270,10 +4431,19 @@
       <c r="F129" s="1" t="n">
         <v>0.98114393</v>
       </c>
+      <c r="G129" s="1" t="n">
+        <v>0.038634032</v>
+      </c>
+      <c r="H129" s="1" t="n">
+        <v>0.16779938</v>
+      </c>
+      <c r="I129" s="1" t="n">
+        <v>0.50409697</v>
+      </c>
     </row>
     <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="0" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="B130" s="0" t="n">
         <v>17</v>
@@ -3290,10 +4460,19 @@
       <c r="F130" s="1" t="n">
         <v>0.38865691</v>
       </c>
+      <c r="G130" s="1" t="n">
+        <v>0.041559088</v>
+      </c>
+      <c r="H130" s="1" t="n">
+        <v>0.19517486</v>
+      </c>
+      <c r="I130" s="1" t="n">
+        <v>0.49687956</v>
+      </c>
     </row>
     <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="0" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="B131" s="0" t="n">
         <v>17</v>
@@ -3310,10 +4489,19 @@
       <c r="F131" s="1" t="n">
         <v>0.48702153</v>
       </c>
+      <c r="G131" s="1" t="n">
+        <v>0.030851</v>
+      </c>
+      <c r="H131" s="1" t="n">
+        <v>0.16263383</v>
+      </c>
+      <c r="I131" s="1" t="n">
+        <v>0.33121954</v>
+      </c>
     </row>
     <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="0" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="B132" s="0" t="n">
         <v>20</v>
@@ -3330,10 +4518,19 @@
       <c r="F132" s="1" t="n">
         <v>0.59598655</v>
       </c>
+      <c r="G132" s="1" t="n">
+        <v>0.034094987</v>
+      </c>
+      <c r="H132" s="1" t="n">
+        <v>0.1837762</v>
+      </c>
+      <c r="I132" s="1" t="n">
+        <v>0.28349069</v>
+      </c>
     </row>
     <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="0" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="B133" s="0" t="n">
         <v>24</v>
@@ -3350,10 +4547,19 @@
       <c r="F133" s="1" t="n">
         <v>0.46781961</v>
       </c>
+      <c r="G133" s="1" t="n">
+        <v>0.023814068</v>
+      </c>
+      <c r="H133" s="1" t="n">
+        <v>0.11262798</v>
+      </c>
+      <c r="I133" s="1" t="n">
+        <v>0.55035728</v>
+      </c>
     </row>
     <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="0" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="B134" s="0" t="n">
         <v>26</v>
@@ -3370,10 +4576,19 @@
       <c r="F134" s="1" t="n">
         <v>0.57093572</v>
       </c>
+      <c r="G134" s="1" t="n">
+        <v>0.050683266</v>
+      </c>
+      <c r="H134" s="1" t="n">
+        <v>0.17322451</v>
+      </c>
+      <c r="I134" s="1" t="n">
+        <v>0.85656896</v>
+      </c>
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="0" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="B135" s="0" t="n">
         <v>28</v>
@@ -3390,10 +4605,19 @@
       <c r="F135" s="1" t="n">
         <v>0.44421384</v>
       </c>
+      <c r="G135" s="1" t="n">
+        <v>0.032619886</v>
+      </c>
+      <c r="H135" s="1" t="n">
+        <v>0.19938077</v>
+      </c>
+      <c r="I135" s="1" t="n">
+        <v>0.37508034</v>
+      </c>
     </row>
     <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="0" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="B136" s="0" t="n">
         <v>28.5</v>
@@ -3410,10 +4634,19 @@
       <c r="F136" s="1" t="n">
         <v>0.2872622</v>
       </c>
+      <c r="G136" s="1" t="n">
+        <v>0.042411041</v>
+      </c>
+      <c r="H136" s="1" t="n">
+        <v>0.1609781</v>
+      </c>
+      <c r="I136" s="1" t="n">
+        <v>0.42649853</v>
+      </c>
     </row>
     <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="0" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="B137" s="0" t="n">
         <v>29</v>
@@ -3430,10 +4663,19 @@
       <c r="F137" s="1" t="n">
         <v>0.25736372</v>
       </c>
+      <c r="G137" s="1" t="n">
+        <v>0.05331979</v>
+      </c>
+      <c r="H137" s="1" t="n">
+        <v>0.14397123</v>
+      </c>
+      <c r="I137" s="1" t="n">
+        <v>0.54619123</v>
+      </c>
     </row>
     <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="0" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="B138" s="0" t="n">
         <v>32</v>
@@ -3450,10 +4692,19 @@
       <c r="F138" s="1" t="n">
         <v>0.16528636</v>
       </c>
+      <c r="G138" s="1" t="n">
+        <v>0.036540964</v>
+      </c>
+      <c r="H138" s="1" t="n">
+        <v>0.16872457</v>
+      </c>
+      <c r="I138" s="1" t="n">
+        <v>0.35304008</v>
+      </c>
     </row>
     <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="0" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="B139" s="0" t="n">
         <v>32</v>
@@ -3470,10 +4721,19 @@
       <c r="F139" s="1" t="n">
         <v>0.20705595</v>
       </c>
+      <c r="G139" s="1" t="n">
+        <v>0.038333642</v>
+      </c>
+      <c r="H139" s="1" t="n">
+        <v>0.21123965</v>
+      </c>
+      <c r="I139" s="1" t="n">
+        <v>0.48946274</v>
+      </c>
     </row>
     <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="0" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="B140" s="0" t="n">
         <v>32</v>
@@ -3490,10 +4750,19 @@
       <c r="F140" s="1" t="n">
         <v>0.68250492</v>
       </c>
+      <c r="G140" s="1" t="n">
+        <v>0.060878402</v>
+      </c>
+      <c r="H140" s="1" t="n">
+        <v>0.19118681</v>
+      </c>
+      <c r="I140" s="1" t="n">
+        <v>0.44480274</v>
+      </c>
     </row>
     <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="0" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="B141" s="0" t="n">
         <v>32</v>
@@ -3510,10 +4779,19 @@
       <c r="F141" s="1" t="n">
         <v>0.27482064</v>
       </c>
+      <c r="G141" s="1" t="n">
+        <v>0.032210877</v>
+      </c>
+      <c r="H141" s="1" t="n">
+        <v>0.21013893</v>
+      </c>
+      <c r="I141" s="1" t="n">
+        <v>0.35570294</v>
+      </c>
     </row>
     <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="0" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="B142" s="0" t="n">
         <v>34</v>
@@ -3530,10 +4808,19 @@
       <c r="F142" s="1" t="n">
         <v>0.23160791</v>
       </c>
+      <c r="G142" s="1" t="n">
+        <v>0.042755336</v>
+      </c>
+      <c r="H142" s="1" t="n">
+        <v>0.15812147</v>
+      </c>
+      <c r="I142" s="1" t="n">
+        <v>0.27602555</v>
+      </c>
     </row>
     <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="0" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="B143" s="0" t="n">
         <v>35</v>
@@ -3550,10 +4837,19 @@
       <c r="F143" s="1" t="n">
         <v>0.70565716</v>
       </c>
+      <c r="G143" s="1" t="n">
+        <v>0.043815663</v>
+      </c>
+      <c r="H143" s="1" t="n">
+        <v>0.18039296</v>
+      </c>
+      <c r="I143" s="1" t="n">
+        <v>0.28660958</v>
+      </c>
     </row>
     <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="B144" s="0" t="n">
         <v>35</v>
@@ -3570,10 +4866,19 @@
       <c r="F144" s="1" t="n">
         <v>0.31306645</v>
       </c>
+      <c r="G144" s="1" t="n">
+        <v>0.03978377</v>
+      </c>
+      <c r="H144" s="1" t="n">
+        <v>0.1484031</v>
+      </c>
+      <c r="I144" s="1" t="n">
+        <v>0.29395487</v>
+      </c>
     </row>
     <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="0" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="B145" s="0" t="n">
         <v>38</v>
@@ -3590,10 +4895,19 @@
       <c r="F145" s="1" t="n">
         <v>0.65060404</v>
       </c>
+      <c r="G145" s="1" t="n">
+        <v>0.028910336</v>
+      </c>
+      <c r="H145" s="1" t="n">
+        <v>0.12245536</v>
+      </c>
+      <c r="I145" s="1" t="n">
+        <v>1.0457589</v>
+      </c>
     </row>
     <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="0" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="B146" s="0" t="n">
         <v>38</v>
@@ -3610,10 +4924,19 @@
       <c r="F146" s="1" t="n">
         <v>0.28056247</v>
       </c>
+      <c r="G146" s="1" t="n">
+        <v>0.042690427</v>
+      </c>
+      <c r="H146" s="1" t="n">
+        <v>0.23532873</v>
+      </c>
+      <c r="I146" s="1" t="n">
+        <v>0.44116561</v>
+      </c>
     </row>
     <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="0" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="B147" s="0" t="n">
         <v>38</v>
@@ -3630,10 +4953,19 @@
       <c r="F147" s="1" t="n">
         <v>0.49956108</v>
       </c>
+      <c r="G147" s="1" t="n">
+        <v>0.042707219</v>
+      </c>
+      <c r="H147" s="1" t="n">
+        <v>0.17798613</v>
+      </c>
+      <c r="I147" s="1" t="n">
+        <v>0.2793452</v>
+      </c>
     </row>
     <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="0" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="B148" s="0" t="n">
         <v>38</v>
@@ -3650,10 +4982,19 @@
       <c r="F148" s="1" t="n">
         <v>0.12917738</v>
       </c>
+      <c r="G148" s="1" t="n">
+        <v>0.052144203</v>
+      </c>
+      <c r="H148" s="1" t="n">
+        <v>0.14118077</v>
+      </c>
+      <c r="I148" s="1" t="n">
+        <v>0.28079535</v>
+      </c>
     </row>
     <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="0" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="B149" s="0" t="n">
         <v>39</v>
@@ -3670,10 +5011,19 @@
       <c r="F149" s="1" t="n">
         <v>0.30457453</v>
       </c>
+      <c r="G149" s="1" t="n">
+        <v>0.034049392</v>
+      </c>
+      <c r="H149" s="1" t="n">
+        <v>0.16426479</v>
+      </c>
+      <c r="I149" s="1" t="n">
+        <v>0.44318466</v>
+      </c>
     </row>
     <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="0" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B150" s="0" t="n">
         <v>39</v>
@@ -3690,10 +5040,19 @@
       <c r="F150" s="1" t="n">
         <v>0.61272035</v>
       </c>
+      <c r="G150" s="1" t="n">
+        <v>0.031838844</v>
+      </c>
+      <c r="H150" s="1" t="n">
+        <v>0.14693928</v>
+      </c>
+      <c r="I150" s="1" t="n">
+        <v>0.38654834</v>
+      </c>
     </row>
     <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="0" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="B151" s="0" t="n">
         <v>40</v>
@@ -3710,10 +5069,19 @@
       <c r="F151" s="1" t="n">
         <v>0.26945462</v>
       </c>
+      <c r="G151" s="1" t="n">
+        <v>0.029443544</v>
+      </c>
+      <c r="H151" s="1" t="n">
+        <v>0.19147388</v>
+      </c>
+      <c r="I151" s="1" t="n">
+        <v>0.34286753</v>
+      </c>
     </row>
     <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="0" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="B152" s="0" t="n">
         <v>41</v>
@@ -3730,10 +5098,19 @@
       <c r="F152" s="1" t="n">
         <v>0.40046715</v>
       </c>
+      <c r="G152" s="1" t="n">
+        <v>0.038648357</v>
+      </c>
+      <c r="H152" s="1" t="n">
+        <v>0.19107329</v>
+      </c>
+      <c r="I152" s="1" t="n">
+        <v>0.43804836</v>
+      </c>
     </row>
     <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="0" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="B153" s="0" t="n">
         <v>42</v>
@@ -3750,10 +5127,19 @@
       <c r="F153" s="1" t="n">
         <v>0.12927257</v>
       </c>
+      <c r="G153" s="1" t="n">
+        <v>0.035776443</v>
+      </c>
+      <c r="H153" s="1" t="n">
+        <v>0.13659232</v>
+      </c>
+      <c r="I153" s="1" t="n">
+        <v>0.50896225</v>
+      </c>
     </row>
     <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="0" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="B154" s="0" t="n">
         <v>45</v>
@@ -3770,10 +5156,19 @@
       <c r="F154" s="1" t="n">
         <v>0.36196063</v>
       </c>
+      <c r="G154" s="1" t="n">
+        <v>0.038034368</v>
+      </c>
+      <c r="H154" s="1" t="n">
+        <v>0.12695781</v>
+      </c>
+      <c r="I154" s="1" t="n">
+        <v>0.46795481</v>
+      </c>
     </row>
     <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="0" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="B155" s="0" t="n">
         <v>46</v>
@@ -3790,10 +5185,19 @@
       <c r="F155" s="1" t="n">
         <v>0.61402546</v>
       </c>
+      <c r="G155" s="1" t="n">
+        <v>0.034602569</v>
+      </c>
+      <c r="H155" s="1" t="n">
+        <v>0.16341206</v>
+      </c>
+      <c r="I155" s="1" t="n">
+        <v>0.27503469</v>
+      </c>
     </row>
     <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="0" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="B156" s="0" t="n">
         <v>51</v>
@@ -3810,10 +5214,19 @@
       <c r="F156" s="1" t="n">
         <v>0.14886616</v>
       </c>
+      <c r="G156" s="1" t="n">
+        <v>0.033600072</v>
+      </c>
+      <c r="H156" s="1" t="n">
+        <v>0.18353739</v>
+      </c>
+      <c r="I156" s="1" t="n">
+        <v>0.65593002</v>
+      </c>
     </row>
     <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="0" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="B157" s="0" t="n">
         <v>53</v>
@@ -3830,10 +5243,19 @@
       <c r="F157" s="1" t="n">
         <v>0.86074848</v>
       </c>
+      <c r="G157" s="1" t="n">
+        <v>0.031007446</v>
+      </c>
+      <c r="H157" s="1" t="n">
+        <v>0.11409219</v>
+      </c>
+      <c r="I157" s="1" t="n">
+        <v>0.88565895</v>
+      </c>
     </row>
     <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="0" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="B158" s="0" t="n">
         <v>55</v>
@@ -3850,10 +5272,19 @@
       <c r="F158" s="1" t="n">
         <v>0.37738761</v>
       </c>
+      <c r="G158" s="1" t="n">
+        <v>0.064183815</v>
+      </c>
+      <c r="H158" s="1" t="n">
+        <v>0.13742817</v>
+      </c>
+      <c r="I158" s="1" t="n">
+        <v>0.39393573</v>
+      </c>
     </row>
     <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="0" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="B159" s="0" t="n">
         <v>59</v>
@@ -3870,10 +5301,19 @@
       <c r="F159" s="1" t="n">
         <v>0.56441072</v>
       </c>
+      <c r="G159" s="1" t="n">
+        <v>0.034919235</v>
+      </c>
+      <c r="H159" s="1" t="n">
+        <v>0.10689398</v>
+      </c>
+      <c r="I159" s="1" t="n">
+        <v>0.71781154</v>
+      </c>
     </row>
     <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="0" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="B160" s="0" t="n">
         <v>61</v>
@@ -3890,10 +5330,19 @@
       <c r="F160" s="1" t="n">
         <v>0.43293835</v>
       </c>
+      <c r="G160" s="1" t="n">
+        <v>0.05236702</v>
+      </c>
+      <c r="H160" s="1" t="n">
+        <v>0.12381825</v>
+      </c>
+      <c r="I160" s="1" t="n">
+        <v>0.45483997</v>
+      </c>
     </row>
     <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="0" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="B161" s="0" t="n">
         <v>62</v>
@@ -3910,10 +5359,19 @@
       <c r="F161" s="1" t="n">
         <v>0.10903675</v>
       </c>
+      <c r="G161" s="1" t="n">
+        <v>0.038055611</v>
+      </c>
+      <c r="H161" s="1" t="n">
+        <v>0.26618358</v>
+      </c>
+      <c r="I161" s="1" t="n">
+        <v>0.83840848</v>
+      </c>
     </row>
     <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="0" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="B162" s="0" t="n">
         <v>63</v>
@@ -3930,10 +5388,19 @@
       <c r="F162" s="1" t="n">
         <v>0.17912502</v>
       </c>
+      <c r="G162" s="1" t="n">
+        <v>0.022427683</v>
+      </c>
+      <c r="H162" s="1" t="n">
+        <v>0.12286687</v>
+      </c>
+      <c r="I162" s="1" t="n">
+        <v>0.45384419</v>
+      </c>
     </row>
     <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="0" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="B163" s="0" t="n">
         <v>63</v>
@@ -3950,10 +5417,19 @@
       <c r="F163" s="1" t="n">
         <v>1.4192525</v>
       </c>
+      <c r="G163" s="1" t="n">
+        <v>0.031456934</v>
+      </c>
+      <c r="H163" s="1" t="n">
+        <v>0.098336875</v>
+      </c>
+      <c r="I163" s="1" t="n">
+        <v>1.179142</v>
+      </c>
     </row>
     <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="0" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="B164" s="0" t="n">
         <v>64</v>
@@ -3970,10 +5446,19 @@
       <c r="F164" s="1" t="n">
         <v>0.39606175</v>
       </c>
+      <c r="G164" s="1" t="n">
+        <v>0.038738152</v>
+      </c>
+      <c r="H164" s="1" t="n">
+        <v>0.19468999</v>
+      </c>
+      <c r="I164" s="1" t="n">
+        <v>0.26510493</v>
+      </c>
     </row>
     <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="0" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="B165" s="0" t="n">
         <v>64</v>
@@ -3990,10 +5475,19 @@
       <c r="F165" s="1" t="n">
         <v>1.0691064</v>
       </c>
+      <c r="G165" s="1" t="n">
+        <v>0.055429968</v>
+      </c>
+      <c r="H165" s="1" t="n">
+        <v>0.12590117</v>
+      </c>
+      <c r="I165" s="1" t="n">
+        <v>0.2945508</v>
+      </c>
     </row>
     <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="0" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="B166" s="0" t="n">
         <v>64</v>
@@ -4010,10 +5504,19 @@
       <c r="F166" s="1" t="n">
         <v>0.60687619</v>
       </c>
+      <c r="G166" s="1" t="n">
+        <v>0.039631101</v>
+      </c>
+      <c r="H166" s="1" t="n">
+        <v>0.12571133</v>
+      </c>
+      <c r="I166" s="1" t="n">
+        <v>0.39313351</v>
+      </c>
     </row>
     <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="0" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="B167" s="0" t="n">
         <v>65</v>
@@ -4030,10 +5533,19 @@
       <c r="F167" s="1" t="n">
         <v>0.86605715</v>
       </c>
+      <c r="G167" s="1" t="n">
+        <v>0.034842131</v>
+      </c>
+      <c r="H167" s="1" t="n">
+        <v>0.13957254</v>
+      </c>
+      <c r="I167" s="1" t="n">
+        <v>1.5290257</v>
+      </c>
     </row>
     <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="0" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="B168" s="0" t="n">
         <v>65</v>
@@ -4050,10 +5562,19 @@
       <c r="F168" s="1" t="n">
         <v>0.077284666</v>
       </c>
+      <c r="G168" s="1" t="n">
+        <v>0.024184632</v>
+      </c>
+      <c r="H168" s="1" t="n">
+        <v>0.17447632</v>
+      </c>
+      <c r="I168" s="1" t="n">
+        <v>0.36455044</v>
+      </c>
     </row>
     <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="0" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="B169" s="0" t="n">
         <v>66</v>
@@ -4070,10 +5591,19 @@
       <c r="F169" s="1" t="n">
         <v>0.1476005</v>
       </c>
+      <c r="G169" s="1" t="n">
+        <v>0.020673484</v>
+      </c>
+      <c r="H169" s="1" t="n">
+        <v>0.17508005</v>
+      </c>
+      <c r="I169" s="1" t="n">
+        <v>0.45395904</v>
+      </c>
     </row>
     <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="0" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="B170" s="0" t="n">
         <v>66</v>
@@ -4090,10 +5620,19 @@
       <c r="F170" s="1" t="n">
         <v>0.14687534</v>
       </c>
+      <c r="G170" s="1" t="n">
+        <v>0.025596447</v>
+      </c>
+      <c r="H170" s="1" t="n">
+        <v>0.16834109</v>
+      </c>
+      <c r="I170" s="1" t="n">
+        <v>0.40907922</v>
+      </c>
     </row>
     <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="0" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="B171" s="0" t="n">
         <v>66</v>
@@ -4110,10 +5649,19 @@
       <c r="F171" s="1" t="n">
         <v>0.35533256</v>
       </c>
+      <c r="G171" s="1" t="n">
+        <v>0.033487681</v>
+      </c>
+      <c r="H171" s="1" t="n">
+        <v>0.15085097</v>
+      </c>
+      <c r="I171" s="1" t="n">
+        <v>0.35983884</v>
+      </c>
     </row>
     <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="0" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="B172" s="0" t="n">
         <v>67</v>
@@ -4130,10 +5678,19 @@
       <c r="F172" s="1" t="n">
         <v>2.0789485</v>
       </c>
+      <c r="G172" s="1" t="n">
+        <v>0.045191211</v>
+      </c>
+      <c r="H172" s="1" t="n">
+        <v>0.1399325</v>
+      </c>
+      <c r="I172" s="1" t="n">
+        <v>0.59932739</v>
+      </c>
     </row>
     <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="0" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="B173" s="0" t="n">
         <v>67</v>
@@ -4150,10 +5707,19 @@
       <c r="F173" s="1" t="n">
         <v>0.14360647</v>
       </c>
+      <c r="G173" s="1" t="n">
+        <v>0.02958803</v>
+      </c>
+      <c r="H173" s="1" t="n">
+        <v>0.13745601</v>
+      </c>
+      <c r="I173" s="1" t="n">
+        <v>0.48239593</v>
+      </c>
     </row>
     <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="0" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="B174" s="0" t="n">
         <v>67</v>
@@ -4170,10 +5736,19 @@
       <c r="F174" s="1" t="n">
         <v>2.2560238</v>
       </c>
+      <c r="G174" s="1" t="n">
+        <v>0.056493752</v>
+      </c>
+      <c r="H174" s="1" t="n">
+        <v>0.12270593</v>
+      </c>
+      <c r="I174" s="1" t="n">
+        <v>0.41437294</v>
+      </c>
     </row>
     <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="0" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="B175" s="0" t="n">
         <v>68</v>
@@ -4190,10 +5765,19 @@
       <c r="F175" s="1" t="n">
         <v>1.1649818</v>
       </c>
+      <c r="G175" s="1" t="n">
+        <v>0.037875605</v>
+      </c>
+      <c r="H175" s="1" t="n">
+        <v>0.134618</v>
+      </c>
+      <c r="I175" s="1" t="n">
+        <v>0.68576264</v>
+      </c>
     </row>
     <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="0" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="B176" s="0" t="n">
         <v>68</v>
@@ -4210,10 +5794,19 @@
       <c r="F176" s="1" t="n">
         <v>0.28269744</v>
       </c>
+      <c r="G176" s="1" t="n">
+        <v>0.02726491</v>
+      </c>
+      <c r="H176" s="1" t="n">
+        <v>0.2007726</v>
+      </c>
+      <c r="I176" s="1" t="n">
+        <v>0.50463398</v>
+      </c>
     </row>
     <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="0" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="B177" s="0" t="n">
         <v>68</v>
@@ -4230,10 +5823,19 @@
       <c r="F177" s="1" t="n">
         <v>0.26548223</v>
       </c>
+      <c r="G177" s="1" t="n">
+        <v>0.033133946</v>
+      </c>
+      <c r="H177" s="1" t="n">
+        <v>0.15091028</v>
+      </c>
+      <c r="I177" s="1" t="n">
+        <v>0.48834961</v>
+      </c>
     </row>
     <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="0" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="B178" s="0" t="n">
         <v>70</v>
@@ -4250,10 +5852,19 @@
       <c r="F178" s="1" t="n">
         <v>0.56926349</v>
       </c>
+      <c r="G178" s="1" t="n">
+        <v>0.03982113</v>
+      </c>
+      <c r="H178" s="1" t="n">
+        <v>0.1202291</v>
+      </c>
+      <c r="I178" s="1" t="n">
+        <v>0.39299821</v>
+      </c>
     </row>
     <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="0" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="B179" s="0" t="n">
         <v>72</v>
@@ -4270,10 +5881,19 @@
       <c r="F179" s="1" t="n">
         <v>0.55473967</v>
       </c>
+      <c r="G179" s="1" t="n">
+        <v>0.070270798</v>
+      </c>
+      <c r="H179" s="1" t="n">
+        <v>0.14602971</v>
+      </c>
+      <c r="I179" s="1" t="n">
+        <v>0.25282408</v>
+      </c>
     </row>
     <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="0" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="B180" s="0" t="n">
         <v>73</v>
@@ -4290,10 +5910,19 @@
       <c r="F180" s="1" t="n">
         <v>0.98243549</v>
       </c>
+      <c r="G180" s="1" t="n">
+        <v>0.082780152</v>
+      </c>
+      <c r="H180" s="1" t="n">
+        <v>0.17667892</v>
+      </c>
+      <c r="I180" s="1" t="n">
+        <v>0.35030866</v>
+      </c>
     </row>
     <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="0" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="B181" s="0" t="n">
         <v>74</v>
@@ -4309,6 +5938,15 @@
       </c>
       <c r="F181" s="1" t="n">
         <v>0.25464357</v>
+      </c>
+      <c r="G181" s="1" t="n">
+        <v>0.023721914</v>
+      </c>
+      <c r="H181" s="1" t="n">
+        <v>0.11696013</v>
+      </c>
+      <c r="I181" s="1" t="n">
+        <v>0.56069662</v>
       </c>
     </row>
   </sheetData>

</xml_diff>